<commit_message>
trying out new math
</commit_message>
<xml_diff>
--- a/MathA_Draft.xlsx
+++ b/MathA_Draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c1410\Documents\GitHub\CoinFlip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B5928C-FD6C-406B-B826-6E629C04F252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C52B552-1BD1-4C2B-8B71-1DFD2FCDC250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5469C1AF-BC43-4C41-9780-4FFCD086E37A}"/>
+    <workbookView xWindow="9090" yWindow="2400" windowWidth="18045" windowHeight="10290" xr2:uid="{5469C1AF-BC43-4C41-9780-4FFCD086E37A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,49 +34,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>Object</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Per 10M</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Total</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x100</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Total of those two</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>=% per block</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chance of getting C decrease for every previous C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chance of getting C on every block (default value)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum value of Chance of getting C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(Multiply those numbers by 100 for % value)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average coin value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average multi value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total weight</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -84,10 +88,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000%"/>
+    <numFmt numFmtId="181" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +116,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -128,6 +140,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -137,7 +186,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -148,6 +197,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,49 +529,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848E8559-D335-490A-ACC8-3493CAC0BFF7}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:H14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -520,28 +584,28 @@
       </c>
       <c r="D2">
         <f>SUM(B:B)</f>
-        <v>9760000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
+        <v>9830000</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3">
         <f>F2/10000000</f>
-        <v>1.5E-6</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="H2">
-        <f>SUM(F:F)</f>
-        <v>240000</v>
-      </c>
-      <c r="J2">
+        <f>SUM(F1:F10)</f>
+        <v>170000</v>
+      </c>
+      <c r="M2">
         <f>D2+H2</f>
         <v>10000000</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -552,18 +616,18 @@
         <f t="shared" ref="C3:C14" si="0">B3/10000000</f>
         <v>1.17E-5</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
+      <c r="E3">
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="G3" s="3">
         <f t="shared" ref="G3:G7" si="1">F3/10000000</f>
-        <v>1.8499999999999999E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>1.15E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>2500</v>
       </c>
@@ -574,18 +638,18 @@
         <f t="shared" si="0"/>
         <v>4.8000000000000001E-5</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
+      <c r="E4">
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" si="1"/>
-        <v>1.8000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>1.2E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -596,152 +660,197 @@
         <f t="shared" si="0"/>
         <v>2.2499999999999999E-4</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
+      <c r="E5">
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>9500</v>
+        <v>9225</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" si="1"/>
-        <v>9.5E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>9.2250000000000003E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>500</v>
       </c>
       <c r="B6">
-        <v>11000</v>
+        <v>16000</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>57500</v>
+        <v>36450</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" si="1"/>
-        <v>5.7499999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>3.6449999999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1">
       <c r="A7">
         <v>250</v>
       </c>
       <c r="B7">
-        <v>27900</v>
+        <v>39900</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>2.7899999999999999E-3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
+        <v>3.9899999999999996E-3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>171000</v>
+        <v>123000</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="1"/>
-        <v>1.7100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>1.23E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" thickBot="1">
       <c r="A8">
         <v>100</v>
       </c>
       <c r="B8">
-        <v>67000</v>
+        <v>85000</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>6.7000000000000002E-3</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:10">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7">
+        <f>SUMPRODUCT(E2:E14, F2:F14)/SUM(F2:F14)</f>
+        <v>2.4516176470588236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>50</v>
       </c>
       <c r="B9">
-        <v>170000</v>
+        <v>130000</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>1.7000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>25</v>
       </c>
       <c r="B10">
-        <v>370000</v>
+        <v>325000</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:10">
+        <v>3.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>770000</v>
+        <v>475000</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12">
-        <v>1350000</v>
+        <v>1450000</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>2400000</v>
+        <v>3000000</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:10">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <f>4600000-8750</f>
-        <v>4591250</v>
+        <v>4306250</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>0.45912500000000001</v>
+        <v>0.43062499999999998</v>
       </c>
       <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1">
+      <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8">
+        <f>SUMPRODUCT(A2:A14, B2:B14)/SUM(B2:B14)</f>
+        <v>6.8638097660223805</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="F17" s="4">
+        <v>1.35E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="F18">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="F19">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>